<commit_message>
prepared testcases and function libraray
</commit_message>
<xml_diff>
--- a/TestInput/HybridData.xlsx
+++ b/TestInput/HybridData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>TCID</t>
   </si>
@@ -79,13 +79,112 @@
   </si>
   <si>
     <t>TestData</t>
+  </si>
+  <si>
+    <t>Launch browser</t>
+  </si>
+  <si>
+    <t>startBrowser</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Launch url in a browser</t>
+  </si>
+  <si>
+    <t>openApplication</t>
+  </si>
+  <si>
+    <t>wait for username</t>
+  </si>
+  <si>
+    <t>waitForElement</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Enter username</t>
+  </si>
+  <si>
+    <t>typeAction</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>wait for password</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>Enter password</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
+    <t>wait for login button</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>click login</t>
+  </si>
+  <si>
+    <t>clickAction</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>//input[@id='password']</t>
+  </si>
+  <si>
+    <t>btnsubmit</t>
+  </si>
+  <si>
+    <t>wait for logout</t>
+  </si>
+  <si>
+    <t>//a[@id='logout']</t>
+  </si>
+  <si>
+    <t>verify title</t>
+  </si>
+  <si>
+    <t>validateTitle</t>
+  </si>
+  <si>
+    <t>Dashboard « Stock Accounting</t>
+  </si>
+  <si>
+    <t>click logout</t>
+  </si>
+  <si>
+    <t>wait for ok button</t>
+  </si>
+  <si>
+    <t>click ok button</t>
+  </si>
+  <si>
+    <t>//button[normalize-space()='OK!']</t>
+  </si>
+  <si>
+    <t>close browser</t>
+  </si>
+  <si>
+    <t>closeBrowser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -104,6 +203,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -136,10 +243,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +545,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,19 +632,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21">
@@ -559,8 +667,264 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
+      <c r="A9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75">
+      <c r="A13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75">
+      <c r="A14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75">
+      <c r="A15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15.75">
+      <c r="A16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Supplier and stockitem testcases
</commit_message>
<xml_diff>
--- a/TestInput/HybridData.xlsx
+++ b/TestInput/HybridData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="390" windowWidth="19815" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="390" windowWidth="19815" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="MasterTestCases" sheetId="1" r:id="rId1"/>
     <sheet name="ApplicationLogin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Suppliers" sheetId="3" r:id="rId3"/>
+    <sheet name="StockItems" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="124">
   <si>
     <t>TCID</t>
   </si>
@@ -178,6 +179,216 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>wait for supplier link</t>
+  </si>
+  <si>
+    <t>//body/div[2]/div[2]/div[1]/div[1]/ul[1]/li[3]/a[1]</t>
+  </si>
+  <si>
+    <t>Click on supplier link</t>
+  </si>
+  <si>
+    <t>wait for add + Icon button</t>
+  </si>
+  <si>
+    <t>(//span[@data-caption='Add'])[1]</t>
+  </si>
+  <si>
+    <t>Click on add icon</t>
+  </si>
+  <si>
+    <t>wait for sopplier number</t>
+  </si>
+  <si>
+    <t>Capture supplier number</t>
+  </si>
+  <si>
+    <t>captureData</t>
+  </si>
+  <si>
+    <t>x_Supplier_Number</t>
+  </si>
+  <si>
+    <t>Enter supplier name</t>
+  </si>
+  <si>
+    <t>Lg suppliers</t>
+  </si>
+  <si>
+    <t>Enter address</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Enter city</t>
+  </si>
+  <si>
+    <t>Kukatpally</t>
+  </si>
+  <si>
+    <t>Enter country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Enter contact person</t>
+  </si>
+  <si>
+    <t>Lg MD</t>
+  </si>
+  <si>
+    <t>Enter phone number</t>
+  </si>
+  <si>
+    <t>54789547878</t>
+  </si>
+  <si>
+    <t>Enter email</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>Enter mobile number</t>
+  </si>
+  <si>
+    <t>5478954562</t>
+  </si>
+  <si>
+    <t>Enter notes</t>
+  </si>
+  <si>
+    <t>Supplying lg goods</t>
+  </si>
+  <si>
+    <t>click add button</t>
+  </si>
+  <si>
+    <t>x_Supplier_Name</t>
+  </si>
+  <si>
+    <t>x_Address</t>
+  </si>
+  <si>
+    <t>x_City</t>
+  </si>
+  <si>
+    <t>x_Country</t>
+  </si>
+  <si>
+    <t>x_Contact_Person</t>
+  </si>
+  <si>
+    <t>x_Phone_Number</t>
+  </si>
+  <si>
+    <t>x__Email</t>
+  </si>
+  <si>
+    <t>x_Mobile_Number</t>
+  </si>
+  <si>
+    <t>x_Notes</t>
+  </si>
+  <si>
+    <t>btnAction</t>
+  </si>
+  <si>
+    <t>//button[contains(text(),'OK!')]</t>
+  </si>
+  <si>
+    <t>Wait for ok button</t>
+  </si>
+  <si>
+    <t>click alert ok button</t>
+  </si>
+  <si>
+    <t>//body/div[17]/div[2]/div[1]/div[4]/div[2]/button[1]</t>
+  </si>
+  <si>
+    <t>validate table</t>
+  </si>
+  <si>
+    <t>suppliertable</t>
+  </si>
+  <si>
+    <t>Locatortype</t>
+  </si>
+  <si>
+    <t>Locatorvalue</t>
+  </si>
+  <si>
+    <t>testData</t>
+  </si>
+  <si>
+    <t>Launch Browser</t>
+  </si>
+  <si>
+    <t>Launch url in Browser</t>
+  </si>
+  <si>
+    <t>wait For Username</t>
+  </si>
+  <si>
+    <t>wait for Login button</t>
+  </si>
+  <si>
+    <t>click login button</t>
+  </si>
+  <si>
+    <t>wait for stock items</t>
+  </si>
+  <si>
+    <t>//*[@id='mi_a_stock_items']</t>
+  </si>
+  <si>
+    <t>Mouse Click</t>
+  </si>
+  <si>
+    <t>mouseOver</t>
+  </si>
+  <si>
+    <t>wait for add button</t>
+  </si>
+  <si>
+    <t>Click on add icon button</t>
+  </si>
+  <si>
+    <t>wait for Category Name</t>
+  </si>
+  <si>
+    <t>x_Category_Name</t>
+  </si>
+  <si>
+    <t>Enter Category Name</t>
+  </si>
+  <si>
+    <t>click on add button</t>
+  </si>
+  <si>
+    <t>wait for confirm ok button</t>
+  </si>
+  <si>
+    <t>click confirm ok button</t>
+  </si>
+  <si>
+    <t>wait for alert ok button</t>
+  </si>
+  <si>
+    <t>(//*[text()='OK'])[6]</t>
+  </si>
+  <si>
+    <t>click on alert ok</t>
+  </si>
+  <si>
+    <t>stockTable</t>
+  </si>
+  <si>
+    <t>Mens</t>
   </si>
 </sst>
 </file>
@@ -231,7 +442,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -239,15 +450,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -589,7 +821,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18.75">
@@ -600,7 +832,7 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18.75">
@@ -634,8 +866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -930,12 +1162,1079 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75">
+      <c r="A2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" ht="15.75">
+      <c r="A4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5">
+        <v>10</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="5">
+        <v>10</v>
+      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
+      <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75">
+      <c r="A10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5">
+        <v>10</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75">
+      <c r="A12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="5">
+        <v>10</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75">
+      <c r="A13" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75">
+      <c r="A14" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="5">
+        <v>10</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="15.75">
+      <c r="A15" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75">
+      <c r="A16" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" s="5">
+        <v>10</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="15.75">
+      <c r="A17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="15.75">
+      <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.75">
+      <c r="A19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="15.75">
+      <c r="A20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="15.75">
+      <c r="A21" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="15.75">
+      <c r="A22" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="15.75">
+      <c r="A23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="15.75">
+      <c r="A24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75">
+      <c r="A25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="15.75">
+      <c r="A26" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="15.75">
+      <c r="A27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75">
+      <c r="A28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="5">
+        <v>10</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="15.75">
+      <c r="A29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" ht="15.75">
+      <c r="A30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="5">
+        <v>10</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.75">
+      <c r="A31" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="15.75">
+      <c r="A32" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="5">
+        <v>6</v>
+      </c>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="15.75">
+      <c r="A33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E24" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="18.75">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75">
+      <c r="A2" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="18.75">
+      <c r="A3" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.75">
+      <c r="A4" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="8">
+        <v>10</v>
+      </c>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="18.75">
+      <c r="A5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" ht="18.75">
+      <c r="A6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="8">
+        <v>10</v>
+      </c>
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="18.75">
+      <c r="A7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75">
+      <c r="A8" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="8">
+        <v>10</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="18.75">
+      <c r="A9" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" ht="18.75">
+      <c r="A10" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="18.75">
+      <c r="A11" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="9">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6" ht="18.75">
+      <c r="A12" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6" ht="18.75">
+      <c r="A13" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="9">
+        <v>10</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6" ht="18.75">
+      <c r="A14" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="18.75">
+      <c r="A15" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="9">
+        <v>10</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6" ht="18.75">
+      <c r="A16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="18.75">
+      <c r="A17" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="9">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="18.75">
+      <c r="A18" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="18.75">
+      <c r="A19" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="9">
+        <v>10</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="18.75">
+      <c r="A20" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="18.75">
+      <c r="A21" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="9">
+        <v>10</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="18.75">
+      <c r="A22" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="18.75">
+      <c r="A23" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="18.75">
+      <c r="A24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>